<commit_message>
cambio de ubicacion PGC
</commit_message>
<xml_diff>
--- a/Desarrollo/EPY/Gestión y Planes/EPY-CP.xlsx
+++ b/Desarrollo/EPY/Gestión y Planes/EPY-CP.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhJBhMy6U4eil1hI+3I9faLWlOxLQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgm5HW019RQOw2irmTjPD1X1lUELw=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -69,6 +69,9 @@
     <t>% de Avance</t>
   </si>
   <si>
+    <t>Recurso</t>
+  </si>
+  <si>
     <t>INICIO</t>
   </si>
   <si>
@@ -78,7 +81,7 @@
     <t>Documento de plan de proyecto</t>
   </si>
   <si>
-    <t>EPY-DPP.odt</t>
+    <t>EPY-DPP.docx</t>
   </si>
   <si>
     <t>Desarrollo del Modelo Lean Canvas</t>
@@ -108,7 +111,7 @@
     <t>Modelo de Casos de Uso del Sistema</t>
   </si>
   <si>
-    <t>EPY-CUS</t>
+    <t>EPY-CUS.xlsx</t>
   </si>
   <si>
     <t>Elaboración de documento de especificación de requisitos</t>
@@ -117,7 +120,7 @@
     <t>Documento de Especificación de Requisitos de Software</t>
   </si>
   <si>
-    <t>EPY-ERS</t>
+    <t>EPY-ERS.xlsx</t>
   </si>
   <si>
     <t>Diseño de la arquitectura del software</t>
@@ -126,7 +129,7 @@
     <t>Documento de Arquitectura de Software</t>
   </si>
   <si>
-    <t>EPY-DAS</t>
+    <t>EPY-DAS.pdf</t>
   </si>
   <si>
     <t>#Hito 02: Analisis</t>
@@ -138,22 +141,25 @@
     <t>Codigo Fuente</t>
   </si>
   <si>
-    <t>Módulo de publicaciones</t>
+    <t>Módulo de usuario</t>
   </si>
   <si>
     <t>Módulo de busqueda</t>
   </si>
   <si>
+    <t>Módulo de pregunta</t>
+  </si>
+  <si>
     <t>Módulo de chat</t>
   </si>
   <si>
     <t>Módulo de pagos</t>
   </si>
   <si>
-    <t>Módulo de notificaciones</t>
-  </si>
-  <si>
-    <t>Módulo de reportes (calificación)</t>
+    <t>Módulo de valoración</t>
+  </si>
+  <si>
+    <t>Módulo de administradores</t>
   </si>
   <si>
     <t>Elaboración de Manual del Usuario</t>
@@ -162,7 +168,7 @@
     <t>Manual de Usuario</t>
   </si>
   <si>
-    <t>EPY_MU</t>
+    <t>EPY-MU.pdf</t>
   </si>
   <si>
     <t>#Hito 03: Desarrollo</t>
@@ -174,7 +180,7 @@
     <t>Documento de Plan de Pruebas</t>
   </si>
   <si>
-    <t>EPY-PPR</t>
+    <t>EPY-PPR.docx</t>
   </si>
   <si>
     <t>Pruebas unitarias de los módulos</t>
@@ -189,7 +195,7 @@
     <t>Documento de resultados de pruebas</t>
   </si>
   <si>
-    <t>EPY-DRP</t>
+    <t>EPY-DRP.docx</t>
   </si>
   <si>
     <t>#Hito 04: Prueba</t>
@@ -258,8 +264,7 @@
       <name val="Docs-Merriweather"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Merriweather"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -267,13 +272,13 @@
     </font>
     <font>
       <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <name val="Merriweather"/>
     </font>
     <font>
       <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Merriweather"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -381,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -461,23 +466,28 @@
     <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="1" fillId="3" fontId="13" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="166" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="8" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -486,20 +496,20 @@
     <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="13" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="12" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="13" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="14" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="8" numFmtId="166" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
@@ -726,7 +736,8 @@
     <col customWidth="1" min="2" max="2" width="53.75"/>
     <col customWidth="1" min="3" max="3" width="37.0"/>
     <col customWidth="1" min="4" max="4" width="17.75"/>
-    <col customWidth="1" min="5" max="6" width="9.38"/>
+    <col customWidth="1" min="5" max="5" width="10.25"/>
+    <col customWidth="1" min="6" max="6" width="10.38"/>
     <col customWidth="1" min="7" max="7" width="16.0"/>
     <col customWidth="1" min="8" max="8" width="10.5"/>
     <col customWidth="1" min="9" max="25" width="9.38"/>
@@ -844,10 +855,13 @@
       <c r="G10" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="H10" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" ht="24.0" customHeight="1">
       <c r="B11" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -857,13 +871,13 @@
     </row>
     <row r="12">
       <c r="B12" s="13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E12" s="16">
         <v>44351.0</v>
@@ -877,13 +891,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E13" s="16">
         <v>44358.0</v>
@@ -897,13 +911,13 @@
     </row>
     <row r="14">
       <c r="B14" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14" s="16">
         <v>44365.0</v>
@@ -917,7 +931,7 @@
     </row>
     <row r="15" ht="26.25" customHeight="1">
       <c r="B15" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -932,13 +946,13 @@
     <row r="16">
       <c r="A16" s="24"/>
       <c r="B16" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E16" s="17">
         <v>44365.0</v>
@@ -946,18 +960,20 @@
       <c r="F16" s="17">
         <v>44372.0</v>
       </c>
-      <c r="G16" s="18"/>
+      <c r="G16" s="18">
+        <v>1.0</v>
+      </c>
       <c r="H16" s="24"/>
     </row>
     <row r="17">
       <c r="B17" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E17" s="17">
         <v>44372.0</v>
@@ -965,17 +981,19 @@
       <c r="F17" s="17">
         <v>44379.0</v>
       </c>
-      <c r="G17" s="29"/>
+      <c r="G17" s="29">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" s="30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="17">
         <v>44372.0</v>
@@ -983,11 +1001,13 @@
       <c r="F18" s="17">
         <v>44379.0</v>
       </c>
-      <c r="G18" s="32"/>
+      <c r="G18" s="32">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="19" ht="25.5" customHeight="1">
       <c r="B19" s="21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -995,14 +1015,16 @@
       <c r="F19" s="22">
         <v>44379.0</v>
       </c>
-      <c r="G19" s="33"/>
+      <c r="G19" s="33">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="17">
@@ -1014,13 +1036,13 @@
       <c r="G20" s="18"/>
     </row>
     <row r="21">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="34"/>
+      <c r="D21" s="35"/>
       <c r="E21" s="17">
         <v>44379.0</v>
       </c>
@@ -1030,96 +1052,96 @@
       <c r="G21" s="18"/>
     </row>
     <row r="22">
-      <c r="A22" s="35"/>
-      <c r="B22" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39">
+      <c r="A22" s="36"/>
+      <c r="B22" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="39"/>
+      <c r="E22" s="40">
+        <v>44379.0</v>
+      </c>
+      <c r="F22" s="40">
         <v>44386.0</v>
       </c>
-      <c r="F22" s="39">
+      <c r="G22" s="41"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="42"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="42"/>
+      <c r="U22" s="42"/>
+      <c r="V22" s="42"/>
+      <c r="W22" s="42"/>
+      <c r="X22" s="42"/>
+      <c r="Y22" s="42"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="B23" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="35"/>
+      <c r="E23" s="17">
+        <v>44386.0</v>
+      </c>
+      <c r="F23" s="17">
         <v>44393.0</v>
       </c>
-      <c r="G22" s="40"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="41"/>
-      <c r="S22" s="41"/>
-      <c r="T22" s="41"/>
-      <c r="U22" s="41"/>
-      <c r="V22" s="41"/>
-      <c r="W22" s="41"/>
-      <c r="X22" s="41"/>
-      <c r="Y22" s="41"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="34"/>
-      <c r="E23" s="17">
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="B24" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="35"/>
+      <c r="E24" s="17">
         <v>44393.0</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F24" s="17">
         <v>44400.0</v>
       </c>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="34"/>
-      <c r="E24" s="17">
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="B25" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="35"/>
+      <c r="E25" s="17">
         <v>44400.0</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F25" s="17">
         <v>44407.0</v>
       </c>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="17">
-        <v>44407.0</v>
-      </c>
-      <c r="F25" s="17">
-        <v>44414.0</v>
-      </c>
       <c r="G25" s="18"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="B26" s="30" t="s">
-        <v>45</v>
+      <c r="B26" s="34" t="s">
+        <v>46</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="34"/>
+        <v>40</v>
+      </c>
+      <c r="D26" s="35"/>
       <c r="E26" s="17">
         <v>44407.0</v>
       </c>
@@ -1129,73 +1151,75 @@
       <c r="G26" s="18"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="30" t="s">
-        <v>46</v>
+      <c r="B27" s="34" t="s">
+        <v>47</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="35"/>
+      <c r="E27" s="17">
+        <v>44407.0</v>
+      </c>
+      <c r="F27" s="17">
+        <v>44414.0</v>
+      </c>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="B28" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="17">
+      <c r="C28" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="17">
         <v>44414.0</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F28" s="17">
         <v>44421.0</v>
       </c>
-      <c r="G27" s="18"/>
-    </row>
-    <row r="28" ht="26.25" customHeight="1">
-      <c r="B28" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="22">
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" ht="26.25" customHeight="1">
+      <c r="B29" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="22">
         <v>44421.0</v>
       </c>
-      <c r="G28" s="33"/>
-    </row>
-    <row r="29">
-      <c r="B29" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="15" t="s">
+      <c r="G29" s="33"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="17">
+      <c r="C30" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="17">
         <v>44421.0</v>
       </c>
-      <c r="F29" s="17">
+      <c r="F30" s="17">
         <v>44428.0</v>
-      </c>
-      <c r="G29" s="18"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="17">
-        <v>44428.0</v>
-      </c>
-      <c r="F30" s="17">
-        <v>44435.0</v>
       </c>
       <c r="G30" s="18"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="B31" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="34"/>
+        <v>55</v>
+      </c>
+      <c r="C31" s="43"/>
+      <c r="D31" s="35"/>
       <c r="E31" s="17">
         <v>44428.0</v>
       </c>
@@ -1205,41 +1229,54 @@
       <c r="G31" s="18"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="C32" s="43"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="17">
+        <v>44428.0</v>
+      </c>
+      <c r="F32" s="17">
+        <v>44435.0</v>
+      </c>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="B33" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="17">
+      <c r="C33" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="17">
         <v>44435.0</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F33" s="17">
         <v>44442.0</v>
       </c>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" ht="27.0" customHeight="1">
-      <c r="B33" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="22">
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" ht="27.0" customHeight="1">
+      <c r="B34" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="22">
         <v>44442.0</v>
       </c>
-      <c r="G33" s="44"/>
-    </row>
-    <row r="34" ht="16.5" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="45"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1"/>
+      <c r="G34" s="45"/>
+    </row>
+    <row r="35" ht="16.5" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="B37" s="46"/>
+    </row>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1"/>
@@ -2180,14 +2217,15 @@
     <row r="975" ht="15.75" customHeight="1"/>
     <row r="976" ht="15.75" customHeight="1"/>
     <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B34:E34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>

</xml_diff>